<commit_message>
Domänenmodell komplett im Pflichtenheft
</commit_message>
<xml_diff>
--- a/Glossar.xlsx
+++ b/Glossar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="114">
   <si>
     <t>RFID</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>Sequence diagramm</t>
+  </si>
+  <si>
+    <t>Core data (Roland zet)</t>
   </si>
 </sst>
 </file>
@@ -701,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -1105,15 +1108,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>105</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>93</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>21</v>
       </c>
@@ -1137,7 +1143,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -1145,7 +1151,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -1153,7 +1159,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>34</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>99</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>101</v>
       </c>
@@ -1193,7 +1199,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>109</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>110</v>
       </c>

</xml_diff>